<commit_message>
new file:   OpenStack/Docs/II.6.6. Multiple Storage back end.md 	modified:   "OpenStack/Images/III. D\341\273\261ng Openstack Stein/New Microsoft Excel Worksheet.xlsx" 	modified:   "OpenStack/Images/III. D\341\273\261ng Openstack Stein/Overview/3.png" 	modified:   OpenStack/README.md
</commit_message>
<xml_diff>
--- a/OpenStack/Images/III. Dựng Openstack Stein/New Microsoft Excel Worksheet.xlsx
+++ b/OpenStack/Images/III. Dựng Openstack Stein/New Microsoft Excel Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\VCC\VCC_Training\OpenStack\Images\III. Dựng Openstack Stein\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF39E25B-268A-4367-97BA-6079F66A2DAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23EE004C-609F-4617-AED2-71AA3DAEA2DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="38">
   <si>
     <t>Bảng địa chỉ IP</t>
   </si>
@@ -117,9 +117,6 @@
     <t>172.16.1.0/24</t>
   </si>
   <si>
-    <t>Block (Cinder)</t>
-  </si>
-  <si>
     <t>Block2 (Nfsserver)</t>
   </si>
   <si>
@@ -127,6 +124,21 @@
   </si>
   <si>
     <t>10.0.0.42</t>
+  </si>
+  <si>
+    <t>Block (Cinder, LVM)</t>
+  </si>
+  <si>
+    <t>Block3 (GFS1)</t>
+  </si>
+  <si>
+    <t>Block2 (GFS2)</t>
+  </si>
+  <si>
+    <t>10.0.0.43</t>
+  </si>
+  <si>
+    <t>10.0.0.44</t>
   </si>
 </sst>
 </file>
@@ -417,69 +429,69 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -761,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="F5:M23"/>
+  <dimension ref="F5:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,65 +790,65 @@
   </cols>
   <sheetData>
     <row r="5" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="25"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="17"/>
     </row>
     <row r="6" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F6" s="13"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="14"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="20"/>
     </row>
     <row r="7" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="17" t="s">
+      <c r="J7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="17" t="s">
+      <c r="L7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="19" t="s">
+      <c r="M7" s="24" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F8" s="22"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="20"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="25"/>
     </row>
     <row r="9" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="26" t="s">
         <v>2</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -862,7 +874,7 @@
       </c>
     </row>
     <row r="10" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F10" s="9"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="2" t="s">
         <v>11</v>
       </c>
@@ -884,7 +896,7 @@
       </c>
     </row>
     <row r="11" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="28" t="s">
         <v>3</v>
       </c>
       <c r="G11" s="3" t="s">
@@ -910,7 +922,7 @@
       </c>
     </row>
     <row r="12" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F12" s="9"/>
+      <c r="F12" s="27"/>
       <c r="G12" s="2" t="s">
         <v>11</v>
       </c>
@@ -932,31 +944,31 @@
       </c>
     </row>
     <row r="13" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F13" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="28" t="s">
+      <c r="F13" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="28" t="s">
+      <c r="H13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="J13" s="29" t="s">
+      <c r="I13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J13" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="K13" s="29" t="s">
+      <c r="K13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L13" s="29"/>
-      <c r="M13" s="30" t="s">
+      <c r="L13" s="9"/>
+      <c r="M13" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F14" s="13"/>
+      <c r="F14" s="18"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -966,31 +978,31 @@
       <c r="M14" s="6"/>
     </row>
     <row r="15" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F15" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="G15" s="29" t="s">
+      <c r="F15" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="29" t="s">
+      <c r="H15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="J15" s="29" t="s">
+      <c r="I15" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J15" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="29" t="s">
+      <c r="K15" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L15" s="29"/>
-      <c r="M15" s="30" t="s">
+      <c r="L15" s="9"/>
+      <c r="M15" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F16" s="15"/>
+      <c r="F16" s="22"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -999,61 +1011,131 @@
       <c r="L16" s="2"/>
       <c r="M16" s="5"/>
     </row>
-    <row r="20" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I20" s="11" t="s">
+    <row r="17" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F17" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17" s="9"/>
+      <c r="M17" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F18" s="22"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="5"/>
+    </row>
+    <row r="19" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F19" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="9"/>
+      <c r="M19" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F20" s="22"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="5"/>
+    </row>
+    <row r="22" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="I22" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="J20" s="12"/>
-      <c r="K20" s="7" t="s">
+      <c r="J22" s="30"/>
+      <c r="K22" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I21" s="13" t="s">
+    <row r="23" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="I23" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J21" s="14"/>
-      <c r="K21" s="6" t="s">
+      <c r="J23" s="20"/>
+      <c r="K23" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I22" s="13" t="s">
+    <row r="24" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="I24" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="J22" s="14"/>
-      <c r="K22" s="6" t="s">
+      <c r="J24" s="20"/>
+      <c r="K24" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I23" s="15" t="s">
+    <row r="25" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="I25" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="J23" s="16"/>
-      <c r="K23" s="5" t="s">
+      <c r="J25" s="23"/>
+      <c r="K25" s="5" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="19">
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="F5:M6"/>
     <mergeCell ref="F13:F14"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="I7:I8"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="F11:F12"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="F15:F16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>